<commit_message>
24th commit without good folder structuring
</commit_message>
<xml_diff>
--- a/2_semester/Расписание 10ПИ 2025.xlsx
+++ b/2_semester/Расписание 10ПИ 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fefse\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_course\2_semester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37411ED0-8D9C-409E-9DC3-ACE0AE59736D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C157DE22-2114-44C3-8D34-7035BE42CF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12345" xr2:uid="{515C897D-804B-4D69-A546-BBBF8DC89014}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{515C897D-804B-4D69-A546-BBBF8DC89014}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="41">
   <si>
     <t>Понедельник</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Лр Конструирование программного обеспечения (413-1)</t>
+  </si>
+  <si>
+    <t>Лк КСИС (200-3а)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
     <xf numFmtId="20" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -528,9 +531,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -568,7 +571,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -674,7 +677,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -816,7 +819,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -826,21 +829,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BDDE03-76F7-4849-8BB1-C0FD01DCB077}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="49.73046875" customWidth="1"/>
-    <col min="3" max="3" width="49.1328125" customWidth="1"/>
+    <col min="2" max="2" width="49.77734375" customWidth="1"/>
+    <col min="3" max="3" width="49.109375" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="49.73046875" customWidth="1"/>
-    <col min="7" max="7" width="49.1328125" customWidth="1"/>
+    <col min="6" max="6" width="49.77734375" customWidth="1"/>
+    <col min="7" max="7" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>3</v>
       </c>
@@ -861,7 +864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>4</v>
       </c>
@@ -874,7 +877,7 @@
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
     </row>
-    <row r="3" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
@@ -887,7 +890,7 @@
       <c r="F3" s="39"/>
       <c r="G3" s="39"/>
     </row>
-    <row r="4" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="30" t="s">
         <v>15</v>
       </c>
@@ -908,7 +911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="30" t="s">
         <v>16</v>
       </c>
@@ -929,7 +932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="30" t="s">
         <v>17</v>
       </c>
@@ -950,7 +953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="32" t="s">
         <v>18</v>
       </c>
@@ -971,7 +974,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="35" t="s">
         <v>5</v>
       </c>
@@ -984,7 +987,7 @@
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
         <v>15</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:7" ht="42.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="30" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:7" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="30" t="s">
         <v>17</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="32" t="s">
         <v>18</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="35" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1080,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="30" t="s">
         <v>15</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="54.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="54.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="30" t="s">
         <v>16</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="30" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="32" t="s">
         <v>18</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="35" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1173,7 @@
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
     </row>
-    <row r="19" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="30" t="s">
         <v>15</v>
       </c>
@@ -1185,13 +1188,13 @@
         <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="30" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="30" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1232,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="32" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="35" t="s">
         <v>8</v>
       </c>
@@ -1259,7 +1262,7 @@
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
     </row>
-    <row r="24" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="30" t="s">
         <v>15</v>
       </c>
@@ -1276,7 +1279,7 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="25" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="30" t="s">
         <v>16</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="30" t="s">
         <v>17</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="32" t="s">
         <v>18</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="35" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1355,7 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
     </row>
-    <row r="29" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="30" t="s">
         <v>15</v>
       </c>
@@ -1365,7 +1368,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="30" t="s">
         <v>16</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="30" t="s">
         <v>17</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="32" t="s">
         <v>18</v>
       </c>
@@ -1424,8 +1427,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>1</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>0.36458333333333331</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8">
         <v>2</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>0.43055555555555558</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>3</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>0.50694444444444442</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12">
         <v>4</v>
       </c>

</xml_diff>